<commit_message>
Fix bug in racf_pct calculation
FIX: Corrected mistake in which I computed % for rows missing an RACF category but meant the opposite.
</commit_message>
<xml_diff>
--- a/data/data-raw/dashboard-data.xlsx
+++ b/data/data-raw/dashboard-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26920"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efernandez\AppData\Local\Box\Box Edit\Documents\VDj4epuP5U+BOFZ_yj255w==\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ECBB0D-B2D9-49BE-A601-AA3002CE219C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{04ECBB0D-B2D9-49BE-A601-AA3002CE219C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A0B60D4-E853-4556-9957-E3D51102300B}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="555" windowWidth="21105" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -167,9 +170,6 @@
     <t>Does workforce development fit under CED or social services? (tina's response: according to the fed: “Workforce development” is an essential component of community economic development in any economic climate, and certainly even more critical during the financial crises we're experiencing today.)</t>
   </si>
   <si>
-    <t>Monroe County DHS</t>
-  </si>
-  <si>
     <t>Complex Care Program</t>
   </si>
   <si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>https://www.monroecounty.gov/files/planning/arpa/July_2023_ARPA_Report_V3_8-22-23_With_Attachments.pdf</t>
+  </si>
+  <si>
+    <t>New with Sept update</t>
   </si>
   <si>
     <t>Cure Violence</t>
@@ -653,6 +656,9 @@
     <t xml:space="preserve">Program that will provide no cost loans or grants to those at or below 200% of the Federal poverty line no cost loans or grants who need transportation to start or keep employment. Support services such as employment coach/mentor and financial literacy. </t>
   </si>
   <si>
+    <t>Monroe County DHS</t>
+  </si>
+  <si>
     <t>https://www.monroecounty.gov/files/news/Referral%20list%20of%20awardees.pdf?v12</t>
   </si>
   <si>
@@ -1222,9 +1228,6 @@
   </si>
   <si>
     <t>Fostering Racial and Ethnic Understanding and Equity</t>
-  </si>
-  <si>
-    <t>New with Sept update</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1237,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2159,13 +2162,13 @@
   <dimension ref="A1:W93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="V69" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="V26" sqref="V26"/>
+      <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="58" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" hidden="1" customWidth="1"/>
@@ -2191,7 +2194,7 @@
     <col min="23" max="23" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="50.1" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2319,7 +2322,7 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="50.1" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2376,13 +2379,13 @@
       </c>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23" s="17" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="17" customFormat="1" ht="50.1" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>25</v>
@@ -2391,7 +2394,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -2413,13 +2416,13 @@
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="R4" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="S4" s="4">
         <v>45160</v>
@@ -2427,11 +2430,11 @@
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5" t="s">
-        <v>395</v>
+        <v>50</v>
       </c>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="50.1" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -2482,7 +2485,7 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="50.1" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>59</v>
@@ -2535,7 +2538,7 @@
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="50.1" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -2590,7 +2593,7 @@
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="50.1" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>66</v>
       </c>
@@ -2605,7 +2608,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>68</v>
@@ -2645,7 +2648,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="50.1" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>71</v>
       </c>
@@ -2700,7 +2703,7 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="50.1" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
@@ -2715,7 +2718,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>79</v>
@@ -2755,7 +2758,7 @@
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="50.1" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>82</v>
       </c>
@@ -2770,7 +2773,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>84</v>
@@ -2810,7 +2813,7 @@
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
     </row>
-    <row r="12" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="50.1" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>88</v>
       </c>
@@ -2863,7 +2866,7 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="11" customFormat="1" ht="50.1" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>94</v>
       </c>
@@ -2922,7 +2925,7 @@
       </c>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="50.1" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>101</v>
       </c>
@@ -2977,7 +2980,7 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="50.1" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>106</v>
       </c>
@@ -3034,7 +3037,7 @@
       </c>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="11" customFormat="1" ht="50.1" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>114</v>
       </c>
@@ -3089,7 +3092,7 @@
       </c>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="50.1" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>119</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>121</v>
@@ -3117,7 +3120,9 @@
       <c r="K17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="13">
+        <v>3009905</v>
+      </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2">
         <v>1</v>
@@ -3142,7 +3147,7 @@
       </c>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="50.1" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>125</v>
       </c>
@@ -3199,7 +3204,7 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="50.1" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>130</v>
       </c>
@@ -3256,7 +3261,7 @@
       </c>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="50.1" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>134</v>
       </c>
@@ -3309,7 +3314,7 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
     </row>
-    <row r="21" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="50.1" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>141</v>
       </c>
@@ -3337,8 +3342,8 @@
       <c r="K21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="3">
-        <v>417225</v>
+      <c r="L21" s="13">
+        <v>5800000</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2">
@@ -3364,7 +3369,7 @@
       </c>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="50.1" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>148</v>
       </c>
@@ -3379,7 +3384,7 @@
         <v>26</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>150</v>
@@ -3421,7 +3426,7 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="50.1" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>154</v>
       </c>
@@ -3480,7 +3485,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="50.1" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>161</v>
       </c>
@@ -3537,7 +3542,7 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="50.1" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>166</v>
       </c>
@@ -3590,7 +3595,7 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="50.1" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>171</v>
       </c>
@@ -3645,7 +3650,7 @@
       </c>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="50.1" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>176</v>
       </c>
@@ -3660,7 +3665,7 @@
         <v>26</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>178</v>
@@ -3702,7 +3707,7 @@
       </c>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="50.1" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>182</v>
       </c>
@@ -3759,7 +3764,7 @@
       </c>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="50.1" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>188</v>
       </c>
@@ -3816,7 +3821,7 @@
       </c>
       <c r="W29" s="2"/>
     </row>
-    <row r="30" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="50.1" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>192</v>
       </c>
@@ -3871,7 +3876,7 @@
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
     </row>
-    <row r="31" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="50.1" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>198</v>
       </c>
@@ -3928,7 +3933,7 @@
       </c>
       <c r="W31" s="2"/>
     </row>
-    <row r="32" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="50.1" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>203</v>
       </c>
@@ -3967,13 +3972,13 @@
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2" t="s">
-        <v>44</v>
+        <v>205</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="S32" s="4">
         <v>45160</v>
@@ -3983,13 +3988,13 @@
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
     </row>
-    <row r="33" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="50.1" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>25</v>
@@ -4022,13 +4027,13 @@
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="S33" s="4">
         <v>45160</v>
@@ -4040,13 +4045,13 @@
       </c>
       <c r="W33" s="2"/>
     </row>
-    <row r="34" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="50.1" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>25</v>
@@ -4058,7 +4063,7 @@
         <v>136</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="2" t="s">
@@ -4079,13 +4084,13 @@
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="S34" s="4">
         <v>45160</v>
@@ -4095,13 +4100,13 @@
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
     </row>
-    <row r="35" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="50.1" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>25</v>
@@ -4110,7 +4115,7 @@
         <v>26</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>79</v>
@@ -4134,13 +4139,13 @@
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="S35" s="4">
         <v>45160</v>
@@ -4150,13 +4155,13 @@
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="50.1" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>25</v>
@@ -4171,7 +4176,7 @@
         <v>54</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -4193,7 +4198,7 @@
         <v>34</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="S36" s="4">
         <v>45160</v>
@@ -4203,13 +4208,13 @@
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
     </row>
-    <row r="37" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="50.1" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>25</v>
@@ -4218,7 +4223,7 @@
         <v>26</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>156</v>
@@ -4242,13 +4247,13 @@
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="S37" s="4">
         <v>45160</v>
@@ -4258,13 +4263,13 @@
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
     </row>
-    <row r="38" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="50.1" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>25</v>
@@ -4297,13 +4302,13 @@
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="S38" s="4">
         <v>45160</v>
@@ -4315,25 +4320,25 @@
       </c>
       <c r="W38" s="2"/>
     </row>
-    <row r="39" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="50.1" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -4352,13 +4357,13 @@
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S39" s="4">
         <v>45160</v>
@@ -4368,28 +4373,28 @@
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
     </row>
-    <row r="40" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="50.1" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -4407,13 +4412,13 @@
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S40" s="4">
         <v>45160</v>
@@ -4423,16 +4428,16 @@
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
     </row>
-    <row r="41" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="50.1" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>26</v>
@@ -4441,7 +4446,7 @@
         <v>38</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -4460,13 +4465,13 @@
       </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S41" s="4">
         <v>45160</v>
@@ -4474,29 +4479,29 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W41" s="2"/>
     </row>
-    <row r="42" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="50.1" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -4515,13 +4520,13 @@
       </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S42" s="4">
         <v>45160</v>
@@ -4531,16 +4536,16 @@
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
     </row>
-    <row r="43" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="50.1" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>26</v>
@@ -4549,7 +4554,7 @@
         <v>38</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="2"/>
@@ -4568,13 +4573,13 @@
       </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S43" s="4">
         <v>45160</v>
@@ -4582,20 +4587,20 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W43" s="2"/>
     </row>
-    <row r="44" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="50.1" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>26</v>
@@ -4604,7 +4609,7 @@
         <v>53</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -4623,13 +4628,13 @@
       </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S44" s="4">
         <v>45160</v>
@@ -4637,20 +4642,20 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W44" s="2"/>
     </row>
-    <row r="45" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="50.1" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>26</v>
@@ -4659,7 +4664,7 @@
         <v>38</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="2" t="s">
@@ -4680,13 +4685,13 @@
       </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S45" s="4">
         <v>45160</v>
@@ -4694,20 +4699,20 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="W45" s="2"/>
     </row>
-    <row r="46" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="50.1" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>26</v>
@@ -4716,11 +4721,11 @@
         <v>136</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>31</v>
@@ -4739,13 +4744,13 @@
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S46" s="4">
         <v>45160</v>
@@ -4755,30 +4760,30 @@
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
     </row>
-    <row r="47" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="50.1" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>32</v>
@@ -4794,13 +4799,13 @@
       </c>
       <c r="O47" s="2"/>
       <c r="P47" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S47" s="4">
         <v>45160</v>
@@ -4808,20 +4813,20 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W47" s="2"/>
     </row>
-    <row r="48" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="50.1" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>26</v>
@@ -4830,7 +4835,7 @@
         <v>38</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -4849,13 +4854,13 @@
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S48" s="4">
         <v>45160</v>
@@ -4863,20 +4868,20 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W48" s="2"/>
     </row>
-    <row r="49" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="50.1" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>26</v>
@@ -4885,7 +4890,7 @@
         <v>38</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="2"/>
@@ -4904,13 +4909,13 @@
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S49" s="4">
         <v>45160</v>
@@ -4918,20 +4923,20 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="50.1" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>26</v>
@@ -4940,7 +4945,7 @@
         <v>27</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -4959,13 +4964,13 @@
       </c>
       <c r="O50" s="2"/>
       <c r="P50" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S50" s="4">
         <v>45160</v>
@@ -4975,28 +4980,28 @@
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
     </row>
-    <row r="51" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="50.1" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -5014,13 +5019,13 @@
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S51" s="4">
         <v>45160</v>
@@ -5030,16 +5035,16 @@
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
     </row>
-    <row r="52" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="50.1" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>26</v>
@@ -5048,7 +5053,7 @@
         <v>38</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -5067,13 +5072,13 @@
       </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S52" s="4">
         <v>45160</v>
@@ -5081,20 +5086,20 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W52" s="2"/>
     </row>
-    <row r="53" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="50.1" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>26</v>
@@ -5103,7 +5108,7 @@
         <v>38</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -5122,13 +5127,13 @@
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S53" s="4">
         <v>45160</v>
@@ -5138,16 +5143,16 @@
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>
     </row>
-    <row r="54" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="50.1" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>26</v>
@@ -5156,7 +5161,7 @@
         <v>53</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -5175,13 +5180,13 @@
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S54" s="4">
         <v>45160</v>
@@ -5189,20 +5194,20 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
       <c r="V54" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W54" s="2"/>
     </row>
-    <row r="55" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="50.1" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>26</v>
@@ -5211,7 +5216,7 @@
         <v>53</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -5230,13 +5235,13 @@
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R55" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S55" s="4">
         <v>45160</v>
@@ -5244,20 +5249,20 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
       <c r="V55" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W55" s="2"/>
     </row>
-    <row r="56" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="50.1" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>26</v>
@@ -5266,7 +5271,7 @@
         <v>53</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -5285,13 +5290,13 @@
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S56" s="4">
         <v>45160</v>
@@ -5299,20 +5304,20 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
       <c r="V56" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W56" s="2"/>
     </row>
-    <row r="57" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="50.1" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>26</v>
@@ -5321,7 +5326,7 @@
         <v>53</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -5340,13 +5345,13 @@
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R57" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S57" s="4">
         <v>45160</v>
@@ -5354,20 +5359,20 @@
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
       <c r="V57" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W57" s="2"/>
     </row>
-    <row r="58" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="50.1" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>26</v>
@@ -5376,7 +5381,7 @@
         <v>53</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -5395,13 +5400,13 @@
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R58" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S58" s="4">
         <v>45160</v>
@@ -5409,20 +5414,20 @@
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
       <c r="V58" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W58" s="2"/>
     </row>
-    <row r="59" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="50.1" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>26</v>
@@ -5431,7 +5436,7 @@
         <v>53</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -5450,13 +5455,13 @@
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R59" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S59" s="4">
         <v>45160</v>
@@ -5464,29 +5469,29 @@
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
       <c r="V59" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="W59" s="2"/>
     </row>
-    <row r="60" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="50.1" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -5505,13 +5510,13 @@
       </c>
       <c r="O60" s="2"/>
       <c r="P60" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S60" s="4">
         <v>45160</v>
@@ -5521,28 +5526,28 @@
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
     </row>
-    <row r="61" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="50.1" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>30</v>
@@ -5564,13 +5569,13 @@
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R61" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S61" s="4">
         <v>45160</v>
@@ -5580,16 +5585,16 @@
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
     </row>
-    <row r="62" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="50.1" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>26</v>
@@ -5601,7 +5606,7 @@
         <v>39</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>40</v>
@@ -5623,13 +5628,13 @@
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q62" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R62" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S62" s="4">
         <v>45160</v>
@@ -5639,16 +5644,16 @@
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
     </row>
-    <row r="63" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="50.1" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>26</v>
@@ -5678,13 +5683,13 @@
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R63" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S63" s="4">
         <v>45160</v>
@@ -5694,16 +5699,16 @@
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
     </row>
-    <row r="64" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="50.1" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>26</v>
@@ -5733,13 +5738,13 @@
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q64" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R64" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S64" s="4">
         <v>45160</v>
@@ -5749,16 +5754,16 @@
       <c r="V64" s="2"/>
       <c r="W64" s="2"/>
     </row>
-    <row r="65" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="50.1" customHeight="1">
       <c r="A65" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>26</v>
@@ -5790,13 +5795,13 @@
       </c>
       <c r="O65" s="2"/>
       <c r="P65" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S65" s="4">
         <v>45160</v>
@@ -5806,16 +5811,16 @@
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
     </row>
-    <row r="66" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="50.1" customHeight="1">
       <c r="A66" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>26</v>
@@ -5824,7 +5829,7 @@
         <v>38</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -5843,13 +5848,13 @@
       </c>
       <c r="O66" s="2"/>
       <c r="P66" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q66" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R66" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S66" s="4">
         <v>45160</v>
@@ -5857,29 +5862,29 @@
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
       <c r="V66" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W66" s="2"/>
     </row>
-    <row r="67" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="50.1" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -5898,13 +5903,13 @@
       </c>
       <c r="O67" s="2"/>
       <c r="P67" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R67" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S67" s="4">
         <v>45160</v>
@@ -5914,16 +5919,16 @@
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
     </row>
-    <row r="68" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="50.1" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>26</v>
@@ -5932,7 +5937,7 @@
         <v>38</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -5951,13 +5956,13 @@
       </c>
       <c r="O68" s="2"/>
       <c r="P68" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R68" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S68" s="4">
         <v>45160</v>
@@ -5965,20 +5970,20 @@
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
       <c r="V68" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W68" s="2"/>
     </row>
-    <row r="69" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="50.1" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>26</v>
@@ -6010,13 +6015,13 @@
       </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q69" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R69" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S69" s="4">
         <v>45160</v>
@@ -6025,28 +6030,28 @@
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
       <c r="W69" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="70" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" ht="50.1" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2" t="s">
@@ -6069,13 +6074,13 @@
       </c>
       <c r="O70" s="2"/>
       <c r="P70" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S70" s="4">
         <v>45160</v>
@@ -6085,16 +6090,16 @@
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
     </row>
-    <row r="71" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="50.1" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>26</v>
@@ -6126,13 +6131,13 @@
       </c>
       <c r="O71" s="2"/>
       <c r="P71" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R71" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S71" s="4">
         <v>45160</v>
@@ -6140,20 +6145,20 @@
       <c r="T71" s="2"/>
       <c r="U71" s="2"/>
       <c r="V71" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="W71" s="2"/>
     </row>
-    <row r="72" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="50.1" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>26</v>
@@ -6162,7 +6167,7 @@
         <v>38</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="2"/>
@@ -6181,13 +6186,13 @@
       </c>
       <c r="O72" s="2"/>
       <c r="P72" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q72" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R72" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S72" s="4">
         <v>45160</v>
@@ -6195,20 +6200,20 @@
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
       <c r="V72" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W72" s="2"/>
     </row>
-    <row r="73" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="50.1" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>26</v>
@@ -6217,14 +6222,14 @@
         <v>38</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>32</v>
@@ -6240,13 +6245,13 @@
       </c>
       <c r="O73" s="2"/>
       <c r="P73" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R73" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S73" s="4">
         <v>45160</v>
@@ -6254,34 +6259,34 @@
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
       <c r="V73" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="W73" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="74" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" ht="50.1" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
@@ -6299,13 +6304,13 @@
       </c>
       <c r="O74" s="2"/>
       <c r="P74" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q74" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S74" s="4">
         <v>45160</v>
@@ -6315,28 +6320,28 @@
       <c r="V74" s="2"/>
       <c r="W74" s="2"/>
     </row>
-    <row r="75" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="50.1" customHeight="1">
       <c r="A75" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
@@ -6354,13 +6359,13 @@
       </c>
       <c r="O75" s="2"/>
       <c r="P75" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S75" s="4">
         <v>45160</v>
@@ -6368,20 +6373,20 @@
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
       <c r="V75" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W75" s="2"/>
     </row>
-    <row r="76" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="50.1" customHeight="1">
       <c r="A76" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>26</v>
@@ -6409,13 +6414,13 @@
       </c>
       <c r="O76" s="2"/>
       <c r="P76" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q76" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R76" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S76" s="4">
         <v>45160</v>
@@ -6425,16 +6430,16 @@
       <c r="V76" s="2"/>
       <c r="W76" s="2"/>
     </row>
-    <row r="77" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="50.1" customHeight="1">
       <c r="A77" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>26</v>
@@ -6446,7 +6451,7 @@
         <v>28</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>30</v>
@@ -6466,13 +6471,13 @@
       </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q77" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R77" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S77" s="4">
         <v>45160</v>
@@ -6482,16 +6487,16 @@
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
     </row>
-    <row r="78" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="50.1" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>26</v>
@@ -6500,11 +6505,11 @@
         <v>136</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H78" s="5"/>
       <c r="I78" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J78" s="5" t="s">
         <v>31</v>
@@ -6523,13 +6528,13 @@
       </c>
       <c r="O78" s="2"/>
       <c r="P78" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q78" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R78" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S78" s="4">
         <v>45160</v>
@@ -6539,16 +6544,16 @@
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
     </row>
-    <row r="79" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="50.1" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>26</v>
@@ -6576,13 +6581,13 @@
       </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q79" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R79" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S79" s="4">
         <v>45160</v>
@@ -6592,16 +6597,16 @@
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
     </row>
-    <row r="80" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="50.1" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>26</v>
@@ -6610,10 +6615,10 @@
         <v>53</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
@@ -6631,13 +6636,13 @@
       </c>
       <c r="O80" s="2"/>
       <c r="P80" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Q80" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R80" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S80" s="4">
         <v>45160</v>
@@ -6647,16 +6652,16 @@
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
     </row>
-    <row r="81" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="50.1" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>26</v>
@@ -6665,7 +6670,7 @@
         <v>38</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H81" s="5"/>
       <c r="I81" s="2"/>
@@ -6684,13 +6689,13 @@
       </c>
       <c r="O81" s="2"/>
       <c r="P81" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q81" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R81" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S81" s="4">
         <v>45160</v>
@@ -6698,20 +6703,20 @@
       <c r="T81" s="2"/>
       <c r="U81" s="2"/>
       <c r="V81" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W81" s="2"/>
     </row>
-    <row r="82" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="50.1" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>26</v>
@@ -6743,13 +6748,13 @@
       </c>
       <c r="O82" s="2"/>
       <c r="P82" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R82" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S82" s="4">
         <v>45160</v>
@@ -6759,28 +6764,28 @@
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
     </row>
-    <row r="83" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="50.1" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>30</v>
@@ -6802,13 +6807,13 @@
       </c>
       <c r="O83" s="2"/>
       <c r="P83" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q83" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R83" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S83" s="4">
         <v>45160</v>
@@ -6818,28 +6823,28 @@
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
     </row>
-    <row r="84" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="50.1" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
@@ -6857,13 +6862,13 @@
       </c>
       <c r="O84" s="2"/>
       <c r="P84" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q84" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S84" s="4">
         <v>45160</v>
@@ -6873,16 +6878,16 @@
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
     </row>
-    <row r="85" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="50.1" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>26</v>
@@ -6914,13 +6919,13 @@
       </c>
       <c r="O85" s="2"/>
       <c r="P85" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R85" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S85" s="4">
         <v>45160</v>
@@ -6931,19 +6936,19 @@
         <v>187</v>
       </c>
       <c r="W85" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="86" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" ht="50.1" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>26</v>
@@ -6973,13 +6978,13 @@
       </c>
       <c r="O86" s="2"/>
       <c r="P86" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q86" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R86" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S86" s="4">
         <v>45160</v>
@@ -6989,16 +6994,16 @@
       <c r="V86" s="2"/>
       <c r="W86" s="2"/>
     </row>
-    <row r="87" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="50.1" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>26</v>
@@ -7030,13 +7035,13 @@
       </c>
       <c r="O87" s="2"/>
       <c r="P87" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q87" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R87" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S87" s="4">
         <v>45160</v>
@@ -7047,19 +7052,19 @@
         <v>43</v>
       </c>
       <c r="W87" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" ht="50.1" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>26</v>
@@ -7091,13 +7096,13 @@
       </c>
       <c r="O88" s="2"/>
       <c r="P88" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Q88" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R88" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S88" s="4">
         <v>45160</v>
@@ -7109,16 +7114,16 @@
       </c>
       <c r="W88" s="2"/>
     </row>
-    <row r="89" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="50.1" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>26</v>
@@ -7150,13 +7155,13 @@
       </c>
       <c r="O89" s="2"/>
       <c r="P89" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R89" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S89" s="4">
         <v>45160</v>
@@ -7168,24 +7173,24 @@
       </c>
       <c r="W89" s="2"/>
     </row>
-    <row r="90" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="60">
       <c r="A90" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F90" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>32</v>
@@ -7200,36 +7205,36 @@
         <v>1</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R90" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S90" s="4">
         <v>45160</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="120">
       <c r="A91" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>32</v>
@@ -7244,27 +7249,27 @@
         <v>1</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R91" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S91" s="4">
         <v>45160</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="60">
       <c r="A92" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>26</v>
@@ -7273,10 +7278,10 @@
         <v>38</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>32</v>
@@ -7291,36 +7296,36 @@
         <v>1</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R92" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S92" s="4">
         <v>45160</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="90">
       <c r="A93" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>32</v>
@@ -7335,13 +7340,13 @@
         <v>1</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R93" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S93" s="4">
         <v>45160</v>
@@ -7393,46 +7398,46 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -7448,31 +7453,31 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -7488,39 +7493,39 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>110</v>
       </c>

</xml_diff>